<commit_message>
forgot to save plot of training data (Map_1_and_7_training_data.xlsx) in last commit...
</commit_message>
<xml_diff>
--- a/Paper/fig/Map_1_and_7_training_data.xlsx
+++ b/Paper/fig/Map_1_and_7_training_data.xlsx
@@ -9,9 +9,6 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
@@ -789,11 +786,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="476404248"/>
-        <c:axId val="476405032"/>
+        <c:axId val="433971440"/>
+        <c:axId val="433971832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="476404248"/>
+        <c:axId val="433971440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -805,13 +802,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="476405032"/>
+        <c:crossAx val="433971832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="476405032"/>
+        <c:axId val="433971832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="15"/>
@@ -849,7 +846,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="476404248"/>
+        <c:crossAx val="433971440"/>
         <c:crossesAt val="-30"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1006,2185 +1003,6 @@
     </cdr:sp>
   </cdr:relSizeAnchor>
 </c:userShapes>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Map 7_all_result"/>
-      <sheetName val="Map 1_all_result"/>
-      <sheetName val="plots"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="O2">
-            <v>0.50016400000000005</v>
-          </cell>
-          <cell r="P2">
-            <v>0.16869317028783903</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="O3">
-            <v>3.0933600000000001E-4</v>
-          </cell>
-          <cell r="P3">
-            <v>2.0640578350739524E-2</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="O4">
-            <v>8.9548899999999996E-4</v>
-          </cell>
-          <cell r="P4">
-            <v>1.2490419626853688E-2</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="O5">
-            <v>8.6065100000000004E-4</v>
-          </cell>
-          <cell r="P5">
-            <v>1.3256001823508511E-2</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="O6">
-            <v>3.4737899999999998E-4</v>
-          </cell>
-          <cell r="P6">
-            <v>1.1600038211171308E-2</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="O7">
-            <v>7.4963199999999997E-4</v>
-          </cell>
-          <cell r="P7">
-            <v>1.0171227690013515E-2</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="O8">
-            <v>3.1356999999999999E-4</v>
-          </cell>
-          <cell r="P8">
-            <v>1.047459638650749E-2</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="O9">
-            <v>1.2918199999999999E-3</v>
-          </cell>
-          <cell r="P9">
-            <v>1.0138253844050794E-2</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="O10">
-            <v>9.2154100000000001E-4</v>
-          </cell>
-          <cell r="P10">
-            <v>1.0299135416923916E-2</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="O11">
-            <v>0.50016400000000005</v>
-          </cell>
-          <cell r="P11">
-            <v>0.16869317028783903</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="O12">
-            <v>0.17458099999999999</v>
-          </cell>
-          <cell r="P12">
-            <v>1.9393761544691034E-2</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="O13">
-            <v>0.14192199999999999</v>
-          </cell>
-          <cell r="P13">
-            <v>2.6181675507928732E-2</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="O14">
-            <v>0.50028799999999995</v>
-          </cell>
-          <cell r="P14">
-            <v>0.17288345743624173</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="O15">
-            <v>8.1287899999999997E-4</v>
-          </cell>
-          <cell r="P15">
-            <v>1.1115717833884185E-2</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="O16">
-            <v>9.9688399999999996E-2</v>
-          </cell>
-          <cell r="P16">
-            <v>1.0520359207774634E-2</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="O17">
-            <v>0.30023899999999998</v>
-          </cell>
-          <cell r="P17">
-            <v>6.5222413112622751E-2</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="O18">
-            <v>0.14227500000000001</v>
-          </cell>
-          <cell r="P18">
-            <v>1.1559118072076279E-2</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="O19">
-            <v>0.17430799999999999</v>
-          </cell>
-          <cell r="P19">
-            <v>1.081694666001258E-2</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="O20">
-            <v>9.9943400000000002E-2</v>
-          </cell>
-          <cell r="P20">
-            <v>1.0318066758731068E-2</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="O21">
-            <v>0.14257700000000001</v>
-          </cell>
-          <cell r="P21">
-            <v>1.1127537421853894E-2</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="O22">
-            <v>0.174594</v>
-          </cell>
-          <cell r="P22">
-            <v>1.8366372399936697E-2</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="O23">
-            <v>0.17496200000000001</v>
-          </cell>
-          <cell r="P23">
-            <v>1.3600866132829974E-2</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="O24">
-            <v>2.78666E-4</v>
-          </cell>
-          <cell r="P24">
-            <v>1.2794335301256491E-2</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="O25">
-            <v>0.50016400000000005</v>
-          </cell>
-          <cell r="P25">
-            <v>0.16869317028783903</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="O26">
-            <v>0.39929999999999999</v>
-          </cell>
-          <cell r="P26">
-            <v>0.10682285418010599</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="O27">
-            <v>0.30026399999999998</v>
-          </cell>
-          <cell r="P27">
-            <v>6.5441350744331453E-2</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="O28">
-            <v>0.20025000000000001</v>
-          </cell>
-          <cell r="P28">
-            <v>3.7818342630925553E-2</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="O29">
-            <v>9.9773600000000004E-2</v>
-          </cell>
-          <cell r="P29">
-            <v>2.2256210943453741E-2</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="O30">
-            <v>5.8090799999999999E-4</v>
-          </cell>
-          <cell r="P30">
-            <v>1.7350245794214941E-2</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="O31">
-            <v>9.9103499999999997E-2</v>
-          </cell>
-          <cell r="P31">
-            <v>1.8161177433465979E-2</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="O32">
-            <v>0.17458099999999999</v>
-          </cell>
-          <cell r="P32">
-            <v>1.9393761544691034E-2</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="O33">
-            <v>0.14333599999999999</v>
-          </cell>
-          <cell r="P33">
-            <v>1.9806213187570091E-2</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="O34">
-            <v>0.17444499999999999</v>
-          </cell>
-          <cell r="P34">
-            <v>1.952814445240475E-2</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="O35">
-            <v>0.100582</v>
-          </cell>
-          <cell r="P35">
-            <v>1.9097748117186168E-2</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="O36">
-            <v>1.20919E-3</v>
-          </cell>
-          <cell r="P36">
-            <v>1.9127019476049723E-2</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="O37">
-            <v>9.9965499999999999E-2</v>
-          </cell>
-          <cell r="P37">
-            <v>1.9615849029888024E-2</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="O38">
-            <v>3.0933600000000001E-4</v>
-          </cell>
-          <cell r="P38">
-            <v>2.0640578350739524E-2</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="O39">
-            <v>0.100503</v>
-          </cell>
-          <cell r="P39">
-            <v>2.2568118761537356E-2</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="O40">
-            <v>0.14192199999999999</v>
-          </cell>
-          <cell r="P40">
-            <v>2.6181675507928732E-2</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="O41">
-            <v>0.49978699999999998</v>
-          </cell>
-          <cell r="P41">
-            <v>0.16485867222441569</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="O42">
-            <v>0.40052900000000002</v>
-          </cell>
-          <cell r="P42">
-            <v>0.10239899209818915</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="O43">
-            <v>0.29982199999999998</v>
-          </cell>
-          <cell r="P43">
-            <v>6.0659282420902003E-2</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="O44">
-            <v>0.200266</v>
-          </cell>
-          <cell r="P44">
-            <v>3.406644932588352E-2</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="O45">
-            <v>9.9753499999999995E-2</v>
-          </cell>
-          <cell r="P45">
-            <v>1.8437793017227113E-2</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="O46">
-            <v>8.9548899999999996E-4</v>
-          </cell>
-          <cell r="P46">
-            <v>1.2490419626853688E-2</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="O47">
-            <v>0.100081</v>
-          </cell>
-          <cell r="P47">
-            <v>1.2460619609557713E-2</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="O48">
-            <v>9.9884299999999995E-2</v>
-          </cell>
-          <cell r="P48">
-            <v>1.3283256993453774E-2</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="O49">
-            <v>9.4324100000000004E-4</v>
-          </cell>
-          <cell r="P49">
-            <v>1.3523996924051205E-2</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="O50">
-            <v>9.9616899999999994E-2</v>
-          </cell>
-          <cell r="P50">
-            <v>1.3349258207528034E-2</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="O51">
-            <v>0.100685</v>
-          </cell>
-          <cell r="P51">
-            <v>1.3161443250167075E-2</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="O52">
-            <v>8.6065100000000004E-4</v>
-          </cell>
-          <cell r="P52">
-            <v>1.3256001823508511E-2</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="O53">
-            <v>0.100914</v>
-          </cell>
-          <cell r="P53">
-            <v>1.352466445821412E-2</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="O54">
-            <v>0.142599</v>
-          </cell>
-          <cell r="P54">
-            <v>1.387734759278581E-2</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="O55">
-            <v>9.9509100000000003E-2</v>
-          </cell>
-          <cell r="P55">
-            <v>1.4570634885075496E-2</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="O56">
-            <v>4.9461500000000001E-4</v>
-          </cell>
-          <cell r="P56">
-            <v>1.6478732281680768E-2</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="O57">
-            <v>0.50028799999999995</v>
-          </cell>
-          <cell r="P57">
-            <v>0.17288345743624173</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="O58">
-            <v>0.399337</v>
-          </cell>
-          <cell r="P58">
-            <v>0.10320809917453461</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="O59">
-            <v>0.29901299999999997</v>
-          </cell>
-          <cell r="P59">
-            <v>5.9961333671399594E-2</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="O60">
-            <v>0.19996900000000001</v>
-          </cell>
-          <cell r="P60">
-            <v>3.3526076988748092E-2</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="O61">
-            <v>0.100533</v>
-          </cell>
-          <cell r="P61">
-            <v>1.8497369303836581E-2</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="O62">
-            <v>6.4971500000000004E-4</v>
-          </cell>
-          <cell r="P62">
-            <v>1.2430922672795927E-2</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="O63">
-            <v>0.100522</v>
-          </cell>
-          <cell r="P63">
-            <v>1.16370274996637E-2</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="O64">
-            <v>0.17436399999999999</v>
-          </cell>
-          <cell r="P64">
-            <v>1.1821140158028775E-2</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="O65">
-            <v>0.14239099999999999</v>
-          </cell>
-          <cell r="P65">
-            <v>1.1645431479945057E-2</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="O66">
-            <v>0.17364099999999999</v>
-          </cell>
-          <cell r="P66">
-            <v>1.1267055700834253E-2</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="O67">
-            <v>0.100387</v>
-          </cell>
-          <cell r="P67">
-            <v>1.1080679591046975E-2</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="O68">
-            <v>1.05646E-3</v>
-          </cell>
-          <cell r="P68">
-            <v>1.1188425571467299E-2</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="O69">
-            <v>9.9560899999999994E-2</v>
-          </cell>
-          <cell r="P69">
-            <v>1.143438975973715E-2</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="O70">
-            <v>3.4737899999999998E-4</v>
-          </cell>
-          <cell r="P70">
-            <v>1.1600038211171308E-2</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="O71">
-            <v>9.9361400000000002E-2</v>
-          </cell>
-          <cell r="P71">
-            <v>1.1833666025667822E-2</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="O72">
-            <v>0.14176</v>
-          </cell>
-          <cell r="P72">
-            <v>1.3016321680945532E-2</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="O73">
-            <v>0.42388199999999998</v>
-          </cell>
-          <cell r="P73">
-            <v>0.10831163565641017</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="O74">
-            <v>0.33159300000000003</v>
-          </cell>
-          <cell r="P74">
-            <v>6.1533785005011478E-2</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="O75">
-            <v>0.24585399999999999</v>
-          </cell>
-          <cell r="P75">
-            <v>3.3860233349538159E-2</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="O76">
-            <v>0.17394100000000001</v>
-          </cell>
-          <cell r="P76">
-            <v>1.8721601256851461E-2</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="O77">
-            <v>0.14262900000000001</v>
-          </cell>
-          <cell r="P77">
-            <v>1.2939858035024466E-2</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="O78">
-            <v>0.17450399999999999</v>
-          </cell>
-          <cell r="P78">
-            <v>1.185531186636159E-2</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="O79">
-            <v>9.9091100000000001E-2</v>
-          </cell>
-          <cell r="P79">
-            <v>1.1631590268814966E-2</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="O80">
-            <v>8.1287899999999997E-4</v>
-          </cell>
-          <cell r="P80">
-            <v>1.1115717833884185E-2</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="O81">
-            <v>9.9688399999999996E-2</v>
-          </cell>
-          <cell r="P81">
-            <v>1.0520359207774634E-2</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="O82">
-            <v>7.4963199999999997E-4</v>
-          </cell>
-          <cell r="P82">
-            <v>1.0171227690013515E-2</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="O83">
-            <v>9.9431099999999994E-2</v>
-          </cell>
-          <cell r="P83">
-            <v>1.0200906678460858E-2</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="O84">
-            <v>9.9508799999999994E-2</v>
-          </cell>
-          <cell r="P84">
-            <v>1.0376796207335148E-2</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="O85">
-            <v>3.1356999999999999E-4</v>
-          </cell>
-          <cell r="P85">
-            <v>1.047459638650749E-2</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="O86">
-            <v>9.9630800000000005E-2</v>
-          </cell>
-          <cell r="P86">
-            <v>1.0652693395719693E-2</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="O87">
-            <v>8.6680500000000001E-4</v>
-          </cell>
-          <cell r="P87">
-            <v>1.1593363661421897E-2</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="O88">
-            <v>0.30023899999999998</v>
-          </cell>
-          <cell r="P88">
-            <v>6.5222413112622751E-2</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="O89">
-            <v>0.20025999999999999</v>
-          </cell>
-          <cell r="P89">
-            <v>3.5092424227202865E-2</v>
-          </cell>
-        </row>
-        <row r="90">
-          <cell r="O90">
-            <v>0.100623</v>
-          </cell>
-          <cell r="P90">
-            <v>1.95937085178223E-2</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="O91">
-            <v>3.70221E-4</v>
-          </cell>
-          <cell r="P91">
-            <v>1.375659123310777E-2</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="O92">
-            <v>0.100262</v>
-          </cell>
-          <cell r="P92">
-            <v>1.2625084417300408E-2</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="O93">
-            <v>0.174154</v>
-          </cell>
-          <cell r="P93">
-            <v>1.2225627014769039E-2</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="O94">
-            <v>0.14227500000000001</v>
-          </cell>
-          <cell r="P94">
-            <v>1.1559118072076279E-2</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="O95">
-            <v>0.17430799999999999</v>
-          </cell>
-          <cell r="P95">
-            <v>1.081694666001258E-2</v>
-          </cell>
-        </row>
-        <row r="96">
-          <cell r="O96">
-            <v>9.9943400000000002E-2</v>
-          </cell>
-          <cell r="P96">
-            <v>1.0318066758731068E-2</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="O97">
-            <v>9.5121600000000001E-5</v>
-          </cell>
-          <cell r="P97">
-            <v>1.0158542791339429E-2</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="O98">
-            <v>9.9357399999999998E-2</v>
-          </cell>
-          <cell r="P98">
-            <v>1.0158880338123583E-2</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="O99">
-            <v>1.2918199999999999E-3</v>
-          </cell>
-          <cell r="P99">
-            <v>1.0138253844050794E-2</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="O100">
-            <v>9.92923E-2</v>
-          </cell>
-          <cell r="P100">
-            <v>1.0222711616320997E-2</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="O101">
-            <v>0.14257700000000001</v>
-          </cell>
-          <cell r="P101">
-            <v>1.1127537421853894E-2</v>
-          </cell>
-        </row>
-        <row r="102">
-          <cell r="O102">
-            <v>0.24526800000000001</v>
-          </cell>
-          <cell r="P102">
-            <v>3.7985287470972372E-2</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="O103">
-            <v>0.173822</v>
-          </cell>
-          <cell r="P103">
-            <v>2.1186193177965145E-2</v>
-          </cell>
-        </row>
-        <row r="104">
-          <cell r="O104">
-            <v>0.14250699999999999</v>
-          </cell>
-          <cell r="P104">
-            <v>1.4805051594520193E-2</v>
-          </cell>
-        </row>
-        <row r="105">
-          <cell r="O105">
-            <v>0.173985</v>
-          </cell>
-          <cell r="P105">
-            <v>1.3319861936385877E-2</v>
-          </cell>
-        </row>
-        <row r="106">
-          <cell r="O106">
-            <v>9.9640000000000006E-2</v>
-          </cell>
-          <cell r="P106">
-            <v>1.2812963080130139E-2</v>
-          </cell>
-        </row>
-        <row r="107">
-          <cell r="O107">
-            <v>1.18717E-3</v>
-          </cell>
-          <cell r="P107">
-            <v>1.2158193306378465E-2</v>
-          </cell>
-        </row>
-        <row r="108">
-          <cell r="O108">
-            <v>9.9587099999999998E-2</v>
-          </cell>
-          <cell r="P108">
-            <v>1.145274865624114E-2</v>
-          </cell>
-        </row>
-        <row r="109">
-          <cell r="O109">
-            <v>0.174404</v>
-          </cell>
-          <cell r="P109">
-            <v>1.0933984098750616E-2</v>
-          </cell>
-        </row>
-        <row r="110">
-          <cell r="O110">
-            <v>0.14236099999999999</v>
-          </cell>
-          <cell r="P110">
-            <v>1.0661733812026538E-2</v>
-          </cell>
-        </row>
-        <row r="111">
-          <cell r="O111">
-            <v>9.8842299999999994E-2</v>
-          </cell>
-          <cell r="P111">
-            <v>1.0492708128344529E-2</v>
-          </cell>
-        </row>
-        <row r="112">
-          <cell r="O112">
-            <v>9.2154100000000001E-4</v>
-          </cell>
-          <cell r="P112">
-            <v>1.0299135416923916E-2</v>
-          </cell>
-        </row>
-        <row r="113">
-          <cell r="O113">
-            <v>9.9165100000000006E-2</v>
-          </cell>
-          <cell r="P113">
-            <v>1.0232910111619148E-2</v>
-          </cell>
-        </row>
-        <row r="114">
-          <cell r="O114">
-            <v>1.0619399999999999E-3</v>
-          </cell>
-          <cell r="P114">
-            <v>1.1010888538613798E-2</v>
-          </cell>
-        </row>
-        <row r="115">
-          <cell r="O115">
-            <v>9.9931400000000004E-2</v>
-          </cell>
-          <cell r="P115">
-            <v>2.5427843718417605E-2</v>
-          </cell>
-        </row>
-        <row r="116">
-          <cell r="O116">
-            <v>1.2949999999999999E-3</v>
-          </cell>
-          <cell r="P116">
-            <v>1.696049395510876E-2</v>
-          </cell>
-        </row>
-        <row r="117">
-          <cell r="O117">
-            <v>9.9361400000000002E-2</v>
-          </cell>
-          <cell r="P117">
-            <v>1.4048021304621728E-2</v>
-          </cell>
-        </row>
-        <row r="118">
-          <cell r="O118">
-            <v>0.17350299999999999</v>
-          </cell>
-          <cell r="P118">
-            <v>1.3013828598164853E-2</v>
-          </cell>
-        </row>
-        <row r="119">
-          <cell r="O119">
-            <v>0.14138200000000001</v>
-          </cell>
-          <cell r="P119">
-            <v>1.2363899801335385E-2</v>
-          </cell>
-        </row>
-        <row r="120">
-          <cell r="O120">
-            <v>0.173959</v>
-          </cell>
-          <cell r="P120">
-            <v>1.1875470507483837E-2</v>
-          </cell>
-        </row>
-        <row r="121">
-          <cell r="O121">
-            <v>0.100018</v>
-          </cell>
-          <cell r="P121">
-            <v>1.1524615352885367E-2</v>
-          </cell>
-        </row>
-        <row r="122">
-          <cell r="O122">
-            <v>8.2929900000000003E-4</v>
-          </cell>
-          <cell r="P122">
-            <v>1.1324621955665656E-2</v>
-          </cell>
-        </row>
-        <row r="123">
-          <cell r="O123">
-            <v>0.10016899999999999</v>
-          </cell>
-          <cell r="P123">
-            <v>1.1102849780375351E-2</v>
-          </cell>
-        </row>
-        <row r="124">
-          <cell r="O124">
-            <v>0.14186099999999999</v>
-          </cell>
-          <cell r="P124">
-            <v>1.0794422980442267E-2</v>
-          </cell>
-        </row>
-        <row r="125">
-          <cell r="O125">
-            <v>0.17397599999999999</v>
-          </cell>
-          <cell r="P125">
-            <v>1.0612731880385199E-2</v>
-          </cell>
-        </row>
-        <row r="126">
-          <cell r="O126">
-            <v>0.142265</v>
-          </cell>
-          <cell r="P126">
-            <v>1.1201499283176822E-2</v>
-          </cell>
-        </row>
-        <row r="127">
-          <cell r="O127">
-            <v>0.174594</v>
-          </cell>
-          <cell r="P127">
-            <v>1.8366372399936697E-2</v>
-          </cell>
-        </row>
-        <row r="128">
-          <cell r="O128">
-            <v>0.10151499999999999</v>
-          </cell>
-          <cell r="P128">
-            <v>1.5750827067199404E-2</v>
-          </cell>
-        </row>
-        <row r="129">
-          <cell r="O129">
-            <v>6.7649799999999999E-4</v>
-          </cell>
-          <cell r="P129">
-            <v>1.4490832730568334E-2</v>
-          </cell>
-        </row>
-        <row r="130">
-          <cell r="O130">
-            <v>9.9837599999999999E-2</v>
-          </cell>
-          <cell r="P130">
-            <v>1.3834634556324367E-2</v>
-          </cell>
-        </row>
-        <row r="131">
-          <cell r="O131">
-            <v>0.17496200000000001</v>
-          </cell>
-          <cell r="P131">
-            <v>1.3600866132829974E-2</v>
-          </cell>
-        </row>
-        <row r="132">
-          <cell r="O132">
-            <v>0.14257900000000001</v>
-          </cell>
-          <cell r="P132">
-            <v>1.3445074128421799E-2</v>
-          </cell>
-        </row>
-        <row r="133">
-          <cell r="O133">
-            <v>0.17448900000000001</v>
-          </cell>
-          <cell r="P133">
-            <v>1.324181393408788E-2</v>
-          </cell>
-        </row>
-        <row r="134">
-          <cell r="O134">
-            <v>0.20077</v>
-          </cell>
-          <cell r="P134">
-            <v>1.2896866324504794E-2</v>
-          </cell>
-        </row>
-        <row r="135">
-          <cell r="O135">
-            <v>9.9248100000000006E-2</v>
-          </cell>
-          <cell r="P135">
-            <v>1.2541237222574143E-2</v>
-          </cell>
-        </row>
-        <row r="136">
-          <cell r="O136">
-            <v>2.78666E-4</v>
-          </cell>
-          <cell r="P136">
-            <v>1.2794335301256491E-2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="2">
-          <cell r="O2">
-            <v>0.50016400000000005</v>
-          </cell>
-          <cell r="P2">
-            <v>9.8206280761888504E-2</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="O3">
-            <v>3.0933600000000001E-4</v>
-          </cell>
-          <cell r="P3">
-            <v>1.8189222269248809E-2</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="O4">
-            <v>8.9548899999999996E-4</v>
-          </cell>
-          <cell r="P4">
-            <v>1.1727050098564519E-2</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="O5">
-            <v>8.6065100000000004E-4</v>
-          </cell>
-          <cell r="P5">
-            <v>1.2566589937520552E-2</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="O6">
-            <v>3.4737899999999998E-4</v>
-          </cell>
-          <cell r="P6">
-            <v>1.0996880062398752E-2</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="O7">
-            <v>7.4963199999999997E-4</v>
-          </cell>
-          <cell r="P7">
-            <v>9.8378296365026277E-3</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="O8">
-            <v>3.1356999999999999E-4</v>
-          </cell>
-          <cell r="P8">
-            <v>1.0053249921801689E-2</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="O9">
-            <v>1.2918199999999999E-3</v>
-          </cell>
-          <cell r="P9">
-            <v>9.7334947945257131E-3</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="O10">
-            <v>9.2154100000000001E-4</v>
-          </cell>
-          <cell r="P10">
-            <v>9.7157669131591046E-3</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="O11">
-            <v>0.50016400000000005</v>
-          </cell>
-          <cell r="P11">
-            <v>9.8206280761888504E-2</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="O12">
-            <v>2.5804300000000001E-4</v>
-          </cell>
-          <cell r="P12">
-            <v>1.511288927929288E-2</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="O13">
-            <v>9.9368099999999995E-4</v>
-          </cell>
-          <cell r="P13">
-            <v>2.0308917208766923E-2</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="O14">
-            <v>0.50028799999999995</v>
-          </cell>
-          <cell r="P14">
-            <v>9.5773266147269998E-2</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="O15">
-            <v>0.100384</v>
-          </cell>
-          <cell r="P15">
-            <v>1.0098685716902506E-2</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="O16">
-            <v>0.100312</v>
-          </cell>
-          <cell r="P16">
-            <v>9.9203394900863832E-3</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="O17">
-            <v>0.30023899999999998</v>
-          </cell>
-          <cell r="P17">
-            <v>4.133878809439108E-2</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="O18">
-            <v>0.10006</v>
-          </cell>
-          <cell r="P18">
-            <v>1.031108944612911E-2</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="O19">
-            <v>0.14266599999999999</v>
-          </cell>
-          <cell r="P19">
-            <v>1.0009799567753205E-2</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="O20">
-            <v>9.9943400000000002E-2</v>
-          </cell>
-          <cell r="P20">
-            <v>9.8180583426804458E-3</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="O21">
-            <v>5.4244099999999995E-4</v>
-          </cell>
-          <cell r="P21">
-            <v>1.0124021540471363E-2</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="O22">
-            <v>4.3848999999999998E-4</v>
-          </cell>
-          <cell r="P22">
-            <v>1.3989687576066126E-2</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="O23">
-            <v>6.4659299999999999E-4</v>
-          </cell>
-          <cell r="P23">
-            <v>1.1003556954226E-2</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="O24">
-            <v>2.78666E-4</v>
-          </cell>
-          <cell r="P24">
-            <v>1.1036187841775583E-2</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="O25">
-            <v>0.50016400000000005</v>
-          </cell>
-          <cell r="P25">
-            <v>9.8206280761888504E-2</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="O26">
-            <v>0.39929999999999999</v>
-          </cell>
-          <cell r="P26">
-            <v>6.6131459242561377E-2</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="O27">
-            <v>0.30026399999999998</v>
-          </cell>
-          <cell r="P27">
-            <v>4.3850571554187735E-2</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="O28">
-            <v>0.20025000000000001</v>
-          </cell>
-          <cell r="P28">
-            <v>2.8525116699608898E-2</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="O29">
-            <v>9.9773600000000004E-2</v>
-          </cell>
-          <cell r="P29">
-            <v>1.9516756259260571E-2</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="O30">
-            <v>5.8090799999999999E-4</v>
-          </cell>
-          <cell r="P30">
-            <v>1.5563905740982776E-2</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="O31">
-            <v>9.3466600000000001E-4</v>
-          </cell>
-          <cell r="P31">
-            <v>1.4804194317832935E-2</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="O32">
-            <v>2.5804300000000001E-4</v>
-          </cell>
-          <cell r="P32">
-            <v>1.511288927929288E-2</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="O33">
-            <v>5.7226800000000002E-4</v>
-          </cell>
-          <cell r="P33">
-            <v>1.5676460532216739E-2</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="O34">
-            <v>6.1221799999999999E-4</v>
-          </cell>
-          <cell r="P34">
-            <v>1.6173676133326438E-2</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="O35">
-            <v>8.6133499999999997E-4</v>
-          </cell>
-          <cell r="P35">
-            <v>1.663322860437522E-2</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="O36">
-            <v>1.20919E-3</v>
-          </cell>
-          <cell r="P36">
-            <v>1.7190226167966435E-2</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="O37">
-            <v>2.4077500000000001E-4</v>
-          </cell>
-          <cell r="P37">
-            <v>1.7708886072162432E-2</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="O38">
-            <v>3.0933600000000001E-4</v>
-          </cell>
-          <cell r="P38">
-            <v>1.8189222269248809E-2</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="O39">
-            <v>5.49936E-4</v>
-          </cell>
-          <cell r="P39">
-            <v>1.8881455338525359E-2</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="O40">
-            <v>9.9368099999999995E-4</v>
-          </cell>
-          <cell r="P40">
-            <v>2.0308917208766923E-2</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="O41">
-            <v>0.49978699999999998</v>
-          </cell>
-          <cell r="P41">
-            <v>9.2574765677843271E-2</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="O42">
-            <v>0.40052900000000002</v>
-          </cell>
-          <cell r="P42">
-            <v>6.0191323692992217E-2</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="O43">
-            <v>0.29982199999999998</v>
-          </cell>
-          <cell r="P43">
-            <v>3.7768471123519984E-2</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="O44">
-            <v>0.200266</v>
-          </cell>
-          <cell r="P44">
-            <v>2.3319756588357943E-2</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="O45">
-            <v>9.9753499999999995E-2</v>
-          </cell>
-          <cell r="P45">
-            <v>1.503006479718846E-2</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="O46">
-            <v>8.9548899999999996E-4</v>
-          </cell>
-          <cell r="P46">
-            <v>1.1727050098564519E-2</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="O47">
-            <v>1.0596399999999999E-3</v>
-          </cell>
-          <cell r="P47">
-            <v>1.1216239142938719E-2</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="O48">
-            <v>8.7347499999999997E-4</v>
-          </cell>
-          <cell r="P48">
-            <v>1.1458636878743727E-2</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="O49">
-            <v>9.4324100000000004E-4</v>
-          </cell>
-          <cell r="P49">
-            <v>1.1759998485794862E-2</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="O50">
-            <v>9.9616899999999994E-2</v>
-          </cell>
-          <cell r="P50">
-            <v>1.2018368963938098E-2</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="O51">
-            <v>7.7828700000000001E-4</v>
-          </cell>
-          <cell r="P51">
-            <v>1.2262752841523571E-2</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="O52">
-            <v>8.6065100000000004E-4</v>
-          </cell>
-          <cell r="P52">
-            <v>1.2566589937520552E-2</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="O53">
-            <v>9.9085900000000005E-2</v>
-          </cell>
-          <cell r="P53">
-            <v>1.2837947239236102E-2</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="O54">
-            <v>4.3525500000000001E-4</v>
-          </cell>
-          <cell r="P54">
-            <v>1.306314832455713E-2</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="O55">
-            <v>5.2878599999999995E-4</v>
-          </cell>
-          <cell r="P55">
-            <v>1.3366241486955121E-2</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="O56">
-            <v>4.9461500000000001E-4</v>
-          </cell>
-          <cell r="P56">
-            <v>1.4184307699364693E-2</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="O57">
-            <v>0.50028799999999995</v>
-          </cell>
-          <cell r="P57">
-            <v>9.5773266147269998E-2</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="O58">
-            <v>0.399337</v>
-          </cell>
-          <cell r="P58">
-            <v>5.9679005188885671E-2</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="O59">
-            <v>0.29901299999999997</v>
-          </cell>
-          <cell r="P59">
-            <v>3.6355579157944663E-2</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="O60">
-            <v>0.19996900000000001</v>
-          </cell>
-          <cell r="P60">
-            <v>2.1984427868712623E-2</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="O61">
-            <v>0.100533</v>
-          </cell>
-          <cell r="P61">
-            <v>1.4101366081789092E-2</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="O62">
-            <v>6.4971500000000004E-4</v>
-          </cell>
-          <cell r="P62">
-            <v>1.1032419669438456E-2</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="O63">
-            <v>1.0128299999999999E-3</v>
-          </cell>
-          <cell r="P63">
-            <v>1.043636307566582E-2</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="O64">
-            <v>9.9977700000000003E-2</v>
-          </cell>
-          <cell r="P64">
-            <v>1.0443907875185735E-2</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="O65">
-            <v>1.9021299999999999E-3</v>
-          </cell>
-          <cell r="P65">
-            <v>1.0447904572344777E-2</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="O66">
-            <v>8.3627599999999995E-4</v>
-          </cell>
-          <cell r="P66">
-            <v>1.0444367850050059E-2</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="O67">
-            <v>4.5548399999999998E-4</v>
-          </cell>
-          <cell r="P67">
-            <v>1.0525135856820357E-2</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="O68">
-            <v>9.9918800000000002E-2</v>
-          </cell>
-          <cell r="P68">
-            <v>1.0685924344694351E-2</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="O69">
-            <v>4.3985200000000002E-4</v>
-          </cell>
-          <cell r="P69">
-            <v>1.086964580547104E-2</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="O70">
-            <v>3.4737899999999998E-4</v>
-          </cell>
-          <cell r="P70">
-            <v>1.0996880062398752E-2</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="O71">
-            <v>9.9361400000000002E-2</v>
-          </cell>
-          <cell r="P71">
-            <v>1.1136870903153219E-2</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="O72">
-            <v>1.2206000000000001E-3</v>
-          </cell>
-          <cell r="P72">
-            <v>1.1685684063646389E-2</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="O73">
-            <v>0.39909699999999998</v>
-          </cell>
-          <cell r="P73">
-            <v>6.3020511889635145E-2</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="O74">
-            <v>0.29937200000000003</v>
-          </cell>
-          <cell r="P74">
-            <v>3.7794376849369218E-2</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="O75">
-            <v>0.20013300000000001</v>
-          </cell>
-          <cell r="P75">
-            <v>2.2546091967823267E-2</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="O76">
-            <v>9.9484799999999998E-2</v>
-          </cell>
-          <cell r="P76">
-            <v>1.4416882992019998E-2</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="O77">
-            <v>9.0254899999999999E-4</v>
-          </cell>
-          <cell r="P77">
-            <v>1.1335378347805434E-2</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="O78">
-            <v>3.9087600000000002E-4</v>
-          </cell>
-          <cell r="P78">
-            <v>1.05391227782172E-2</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="O79">
-            <v>1.07879E-3</v>
-          </cell>
-          <cell r="P79">
-            <v>1.031270349231996E-2</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="O80">
-            <v>0.100384</v>
-          </cell>
-          <cell r="P80">
-            <v>1.0098685716902506E-2</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="O81">
-            <v>0.100312</v>
-          </cell>
-          <cell r="P81">
-            <v>9.9203394900863832E-3</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="O82">
-            <v>7.4963199999999997E-4</v>
-          </cell>
-          <cell r="P82">
-            <v>9.8378296365026277E-3</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="O83">
-            <v>6.5129599999999999E-4</v>
-          </cell>
-          <cell r="P83">
-            <v>9.9012390761289044E-3</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="O84">
-            <v>9.9508799999999994E-2</v>
-          </cell>
-          <cell r="P84">
-            <v>9.9985021836585617E-3</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="O85">
-            <v>3.1356999999999999E-4</v>
-          </cell>
-          <cell r="P85">
-            <v>1.0053249921801689E-2</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="O86">
-            <v>4.7970599999999999E-4</v>
-          </cell>
-          <cell r="P86">
-            <v>1.0156362577954641E-2</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="O87">
-            <v>8.6680500000000001E-4</v>
-          </cell>
-          <cell r="P87">
-            <v>1.0550970713451039E-2</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="O88">
-            <v>0.30023899999999998</v>
-          </cell>
-          <cell r="P88">
-            <v>4.133878809439108E-2</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="O89">
-            <v>0.20025999999999999</v>
-          </cell>
-          <cell r="P89">
-            <v>2.4306228871110051E-2</v>
-          </cell>
-        </row>
-        <row r="90">
-          <cell r="O90">
-            <v>0.100623</v>
-          </cell>
-          <cell r="P90">
-            <v>1.5555742726559419E-2</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="O91">
-            <v>3.70221E-4</v>
-          </cell>
-          <cell r="P91">
-            <v>1.2059806268172399E-2</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="O92">
-            <v>9.9738599999999997E-2</v>
-          </cell>
-          <cell r="P92">
-            <v>1.1051601390754062E-2</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="O93">
-            <v>2.29867E-4</v>
-          </cell>
-          <cell r="P93">
-            <v>1.0653085517030285E-2</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="O94">
-            <v>0.10006</v>
-          </cell>
-          <cell r="P94">
-            <v>1.031108944612911E-2</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="O95">
-            <v>0.14266599999999999</v>
-          </cell>
-          <cell r="P95">
-            <v>1.0009799567753205E-2</v>
-          </cell>
-        </row>
-        <row r="96">
-          <cell r="O96">
-            <v>9.9943400000000002E-2</v>
-          </cell>
-          <cell r="P96">
-            <v>9.8180583426804458E-3</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="O97">
-            <v>9.5121600000000001E-5</v>
-          </cell>
-          <cell r="P97">
-            <v>9.7554163068046089E-3</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="O98">
-            <v>1.14119E-3</v>
-          </cell>
-          <cell r="P98">
-            <v>9.7478183994477094E-3</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="O99">
-            <v>1.2918199999999999E-3</v>
-          </cell>
-          <cell r="P99">
-            <v>9.7334947945257131E-3</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="O100">
-            <v>9.92923E-2</v>
-          </cell>
-          <cell r="P100">
-            <v>9.7648819711522328E-3</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="O101">
-            <v>5.4244099999999995E-4</v>
-          </cell>
-          <cell r="P101">
-            <v>1.0124021540471363E-2</v>
-          </cell>
-        </row>
-        <row r="102">
-          <cell r="O102">
-            <v>0.199683</v>
-          </cell>
-          <cell r="P102">
-            <v>2.7003933845909874E-2</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="O103">
-            <v>9.9440299999999995E-2</v>
-          </cell>
-          <cell r="P103">
-            <v>1.7041151893616064E-2</v>
-          </cell>
-        </row>
-        <row r="104">
-          <cell r="O104">
-            <v>3.8285199999999999E-4</v>
-          </cell>
-          <cell r="P104">
-            <v>1.2950521157842692E-2</v>
-          </cell>
-        </row>
-        <row r="105">
-          <cell r="O105">
-            <v>4.9466500000000004E-4</v>
-          </cell>
-          <cell r="P105">
-            <v>1.1626760589056729E-2</v>
-          </cell>
-        </row>
-        <row r="106">
-          <cell r="O106">
-            <v>9.9640000000000006E-2</v>
-          </cell>
-          <cell r="P106">
-            <v>1.1104620109493925E-2</v>
-          </cell>
-        </row>
-        <row r="107">
-          <cell r="O107">
-            <v>1.18717E-3</v>
-          </cell>
-          <cell r="P107">
-            <v>1.0703622761781759E-2</v>
-          </cell>
-        </row>
-        <row r="108">
-          <cell r="O108">
-            <v>1.1419100000000001E-3</v>
-          </cell>
-          <cell r="P108">
-            <v>1.034361056512819E-2</v>
-          </cell>
-        </row>
-        <row r="109">
-          <cell r="O109">
-            <v>4.6800599999999998E-4</v>
-          </cell>
-          <cell r="P109">
-            <v>1.0078184929486044E-2</v>
-          </cell>
-        </row>
-        <row r="110">
-          <cell r="O110">
-            <v>8.7600700000000004E-4</v>
-          </cell>
-          <cell r="P110">
-            <v>9.9201057202189923E-3</v>
-          </cell>
-        </row>
-        <row r="111">
-          <cell r="O111">
-            <v>9.8842299999999994E-2</v>
-          </cell>
-          <cell r="P111">
-            <v>9.8086123267601341E-3</v>
-          </cell>
-        </row>
-        <row r="112">
-          <cell r="O112">
-            <v>9.2154100000000001E-4</v>
-          </cell>
-          <cell r="P112">
-            <v>9.7157669131591046E-3</v>
-          </cell>
-        </row>
-        <row r="113">
-          <cell r="O113">
-            <v>1.6831999999999999E-3</v>
-          </cell>
-          <cell r="P113">
-            <v>9.6958047233786631E-3</v>
-          </cell>
-        </row>
-        <row r="114">
-          <cell r="O114">
-            <v>1.0619399999999999E-3</v>
-          </cell>
-          <cell r="P114">
-            <v>1.003926107708843E-2</v>
-          </cell>
-        </row>
-        <row r="115">
-          <cell r="O115">
-            <v>9.9931400000000004E-2</v>
-          </cell>
-          <cell r="P115">
-            <v>1.936398013167704E-2</v>
-          </cell>
-        </row>
-        <row r="116">
-          <cell r="O116">
-            <v>1.2949999999999999E-3</v>
-          </cell>
-          <cell r="P116">
-            <v>1.4171204989175555E-2</v>
-          </cell>
-        </row>
-        <row r="117">
-          <cell r="O117">
-            <v>8.1150999999999999E-4</v>
-          </cell>
-          <cell r="P117">
-            <v>1.2224464168804267E-2</v>
-          </cell>
-        </row>
-        <row r="118">
-          <cell r="O118">
-            <v>8.7995E-4</v>
-          </cell>
-          <cell r="P118">
-            <v>1.1445202116278237E-2</v>
-          </cell>
-        </row>
-        <row r="119">
-          <cell r="O119">
-            <v>1.4878000000000001E-3</v>
-          </cell>
-          <cell r="P119">
-            <v>1.0983293256289705E-2</v>
-          </cell>
-        </row>
-        <row r="120">
-          <cell r="O120">
-            <v>6.9592500000000002E-4</v>
-          </cell>
-          <cell r="P120">
-            <v>1.0644400862045085E-2</v>
-          </cell>
-        </row>
-        <row r="121">
-          <cell r="O121">
-            <v>9.9986099999999994E-2</v>
-          </cell>
-          <cell r="P121">
-            <v>1.0341526566759249E-2</v>
-          </cell>
-        </row>
-        <row r="122">
-          <cell r="O122">
-            <v>8.2929900000000003E-4</v>
-          </cell>
-          <cell r="P122">
-            <v>1.0130835707043885E-2</v>
-          </cell>
-        </row>
-        <row r="123">
-          <cell r="O123">
-            <v>8.0237899999999998E-4</v>
-          </cell>
-          <cell r="P123">
-            <v>9.9580546629270874E-3</v>
-          </cell>
-        </row>
-        <row r="124">
-          <cell r="O124">
-            <v>1.0204299999999999E-3</v>
-          </cell>
-          <cell r="P124">
-            <v>9.8217667777901578E-3</v>
-          </cell>
-        </row>
-        <row r="125">
-          <cell r="O125">
-            <v>9.9300799999999995E-2</v>
-          </cell>
-          <cell r="P125">
-            <v>9.8337082294769704E-3</v>
-          </cell>
-        </row>
-        <row r="126">
-          <cell r="O126">
-            <v>1.28502E-3</v>
-          </cell>
-          <cell r="P126">
-            <v>1.0233220703424972E-2</v>
-          </cell>
-        </row>
-        <row r="127">
-          <cell r="O127">
-            <v>4.3848999999999998E-4</v>
-          </cell>
-          <cell r="P127">
-            <v>1.3989687576066126E-2</v>
-          </cell>
-        </row>
-        <row r="128">
-          <cell r="O128">
-            <v>1.6383999999999999E-3</v>
-          </cell>
-          <cell r="P128">
-            <v>1.2603536826086821E-2</v>
-          </cell>
-        </row>
-        <row r="129">
-          <cell r="O129">
-            <v>6.7649799999999999E-4</v>
-          </cell>
-          <cell r="P129">
-            <v>1.1860758662245943E-2</v>
-          </cell>
-        </row>
-        <row r="130">
-          <cell r="O130">
-            <v>1.1107700000000001E-3</v>
-          </cell>
-          <cell r="P130">
-            <v>1.1360810043696948E-2</v>
-          </cell>
-        </row>
-        <row r="131">
-          <cell r="O131">
-            <v>6.4659299999999999E-4</v>
-          </cell>
-          <cell r="P131">
-            <v>1.1003556954226E-2</v>
-          </cell>
-        </row>
-        <row r="132">
-          <cell r="O132">
-            <v>3.4654599999999999E-4</v>
-          </cell>
-          <cell r="P132">
-            <v>1.0751386544489991E-2</v>
-          </cell>
-        </row>
-        <row r="133">
-          <cell r="O133">
-            <v>2.4636200000000002E-4</v>
-          </cell>
-          <cell r="P133">
-            <v>1.0556717090968721E-2</v>
-          </cell>
-        </row>
-        <row r="134">
-          <cell r="O134">
-            <v>8.3269699999999997E-4</v>
-          </cell>
-          <cell r="P134">
-            <v>1.0460373411049287E-2</v>
-          </cell>
-        </row>
-        <row r="135">
-          <cell r="O135">
-            <v>7.5375099999999999E-4</v>
-          </cell>
-          <cell r="P135">
-            <v>1.0534378600237339E-2</v>
-          </cell>
-        </row>
-        <row r="136">
-          <cell r="O136">
-            <v>2.78666E-4</v>
-          </cell>
-          <cell r="P136">
-            <v>1.1036187841775583E-2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3477,7 +1295,7 @@
   <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3492,6 +1310,10 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
+      <c r="G1">
+        <f>MIN(G3:G26)</f>
+        <v>-15.022134911463516</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3571,11 +1393,11 @@
         <v>79.988141734426193</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G67" si="2">(E4-32)/1.8</f>
+        <f t="shared" ref="G4:G26" si="2">(E4-32)/1.8</f>
         <v>1.6999238798422784</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H67" si="3">(F4-32)/1.8</f>
+        <f t="shared" ref="H4:H26" si="3">(F4-32)/1.8</f>
         <v>26.660078741347885</v>
       </c>
     </row>

</xml_diff>